<commit_message>
Refactor code to create a new sheet in the Excel file and compare two different Excel files.
</commit_message>
<xml_diff>
--- a/z.xlsx
+++ b/z.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="zz" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="xx" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="s1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="s2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14849,14 +14849,369 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Service Item ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Item Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Folder</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Folder (after)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Item Title</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Item Title (after)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Shared With</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Shared With (after)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Layer Title</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Layer Title (after)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Layer Visibility</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Layer Visibility (after)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Layer Item ID</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Layer Item ID (after)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Popup Title</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Popup Title (after)</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Form Configured</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Form Configured (after)</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>FormField</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>FormField (after)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>FormLabel</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>FormLabel (after)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>FormFieldEditable</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>FormFieldEditable (after)</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>FormFieldInputType</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>FormFieldInputType (after)</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Expression</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Expression (after)</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>FormFieldRequired</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>FormFieldRequired (after)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Offline Status</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Offline Status (after)</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Delete Protection</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Delete Protection (after)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>c7654927cf554c9490fe639178351fb9</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Web Map</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>ARM 2023 Space</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>ARM 2023 Space Test</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>LP_TestMap</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>LP_TestMap</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>LandPlanner_Area_Dev2023</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>LandPlanner_Area_Dev2023</t>
+        </is>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>c49a708cc0ac4ca1a634228ca7de0bf6</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>c49a708cc0ac4ca1a634228ca7de0bf6</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>{OBJECTID}</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>{OBJECTID}</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Not Configured</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Not Configured</t>
+        </is>
+      </c>
+      <c r="AG2" s="2" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="AH2" s="2" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>6003d30a5f06445897ac7facd7287480</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Web Map</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ARM_b Transmission Roads</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ARM_b Transmission Roads</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>All Electric Transmission Operations Map</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>All Electric Transmission Operations Map</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Workcenter</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Workcenter</t>
+        </is>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>c1c831c25b44444b9491df15c56ce7bc</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>c1c831c25b44444b9491df15c56ce7bc</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Workcenter: {WORKCENTER_ARM}</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Workcenter: {WORKCENTER_ARM}</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Not Configured</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Not Configured</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor code to create a new sheet in the Excel file and update user prompt for comparing two new excel files.
</commit_message>
<xml_diff>
--- a/z.xlsx
+++ b/z.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="s1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="s2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14841,377 +14840,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AH3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Service Item ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Item Type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Folder</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Folder (after)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Item Title</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Item Title (after)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Shared With</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Shared With (after)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Layer Title</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Layer Title (after)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Layer Visibility</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Layer Visibility (after)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Layer Item ID</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Layer Item ID (after)</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Popup Title</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Popup Title (after)</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Form Configured</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Form Configured (after)</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>FormField</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>FormField (after)</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>FormLabel</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>FormLabel (after)</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>FormFieldEditable</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>FormFieldEditable (after)</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>FormFieldInputType</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>FormFieldInputType (after)</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Expression</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Expression (after)</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>FormFieldRequired</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>FormFieldRequired (after)</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Offline Status</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Offline Status (after)</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Delete Protection</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Delete Protection (after)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>c7654927cf554c9490fe639178351fb9</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Web Map</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>ARM 2023 Space</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>ARM 2023 Space Test</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>LP_TestMap</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>LP_TestMap</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>LandPlanner_Area_Dev2023</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>LandPlanner_Area_Dev2023</t>
-        </is>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>c49a708cc0ac4ca1a634228ca7de0bf6</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>c49a708cc0ac4ca1a634228ca7de0bf6</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>{OBJECTID}</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>{OBJECTID}</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Not Configured</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Not Configured</t>
-        </is>
-      </c>
-      <c r="AG2" s="2" t="inlineStr">
-        <is>
-          <t>On</t>
-        </is>
-      </c>
-      <c r="AH2" s="2" t="inlineStr">
-        <is>
-          <t>Off</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>6003d30a5f06445897ac7facd7287480</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Web Map</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ARM_b Transmission Roads</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ARM_b Transmission Roads</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>All Electric Transmission Operations Map</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>All Electric Transmission Operations Map</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Workcenter</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Workcenter</t>
-        </is>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>c1c831c25b44444b9491df15c56ce7bc</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>c1c831c25b44444b9491df15c56ce7bc</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Workcenter: {WORKCENTER_ARM}</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Workcenter: {WORKCENTER_ARM}</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Not Configured</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Not Configured</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>Off</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>Off</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>